<commit_message>
Creating profile 1.0 without working by lines on xlsx 13.02.25
</commit_message>
<xml_diff>
--- a/data/output.xlsx
+++ b/data/output.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,15 +25,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -46,23 +53,34 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +445,11 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -451,17 +469,17 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>wrickkorayd8@outlook.com</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>JPk52IAG2T</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>6080475e67e2258b6bd1701f763c2b39a3243293</t>
         </is>

</xml_diff>